<commit_message>
added power button and generated board
added power button and generated board
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lara Ni\Desktop\numitron clock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lara Ni\Desktop\numi_clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="numitron_tube_clock" sheetId="1" r:id="rId1"/>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>